<commit_message>
Update the example file
</commit_message>
<xml_diff>
--- a/inst/demo/expdb_example.xlsx
+++ b/inst/demo/expdb_example.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B9D1FD-740D-455B-88D3-DC72C862D045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996E2AE6-E6E0-4FE2-9E02-213D76B8A161}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14160" tabRatio="813" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14160" tabRatio="813" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="12" r:id="rId1"/>
@@ -29,12 +29,22 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="86">
   <si>
     <t>name</t>
   </si>
@@ -51,18 +61,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>TrialCode</t>
   </si>
   <si>
@@ -172,6 +170,138 @@
   </si>
   <si>
     <t>Biomass</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>Demo data</t>
+  </si>
+  <si>
+    <t>Create the demo file</t>
+  </si>
+  <si>
+    <t>demo@example.com</t>
+  </si>
+  <si>
+    <t>Demo user</t>
+  </si>
+  <si>
+    <t>F_Yield</t>
+  </si>
+  <si>
+    <t>Crop</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>t/ha</t>
+  </si>
+  <si>
+    <t>Crop yield</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>MeasurementIndex</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>P_ZadoksScore</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>Zadoks score</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>O_HaunIndex</t>
+  </si>
+  <si>
+    <t>Organ</t>
+  </si>
+  <si>
+    <t>Haun index</t>
+  </si>
+  <si>
+    <t>Haun index for stem (normally for main stem)</t>
+  </si>
+  <si>
+    <t>P_PlantHeight</t>
+  </si>
+  <si>
+    <t>Plant height</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Gatton</t>
+  </si>
+  <si>
+    <t>Gatton Research Station</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>gatton-2015-daily.met</t>
+  </si>
+  <si>
+    <t>The weather station in Gatton</t>
+  </si>
+  <si>
+    <t>gatton-15-daily</t>
+  </si>
+  <si>
+    <t>Suntop</t>
+  </si>
+  <si>
+    <t>Spitfire</t>
+  </si>
+  <si>
+    <t>Hartog</t>
+  </si>
+  <si>
+    <t>DemoResearcher</t>
+  </si>
+  <si>
+    <t>DemoSource</t>
+  </si>
+  <si>
+    <t>15Trial-1</t>
+  </si>
+  <si>
+    <t>15Trial-2</t>
+  </si>
+  <si>
+    <t>Demo trial sowing 1</t>
+  </si>
+  <si>
+    <t>Demo trial sowing 2</t>
+  </si>
+  <si>
+    <t>gatton-15-hourly</t>
+  </si>
+  <si>
+    <t>gatton-2015-hourly.met</t>
   </si>
 </sst>
 </file>
@@ -181,7 +311,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-C09]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,6 +471,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -639,7 +777,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -688,8 +826,9 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -724,8 +863,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="45"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
@@ -759,6 +900,7 @@
     <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
     <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
@@ -1106,12 +1248,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1126,10 +1268,21 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1169,37 +1322,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="G1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>36</v>
-      </c>
       <c r="K1" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="12:18" x14ac:dyDescent="0.35">
@@ -1419,43 +1572,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>41</v>
-      </c>
       <c r="L1" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="11:17" x14ac:dyDescent="0.35">
@@ -1648,10 +1801,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF168F87-6153-46F1-B31A-82AB581E3C1A}">
   <dimension ref="A1:Q205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G21" sqref="G21"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1674,34 +1827,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="G1" s="10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="10:16" x14ac:dyDescent="0.35">
@@ -1907,13 +2060,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1958,16 +2111,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1989,7 +2142,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2001,14 +2154,19 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5"/>
+      <c r="A2" s="5">
+        <v>44259</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
@@ -2024,10 +2182,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2045,21 +2203,35 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{51CBA857-8B83-4B3B-AB35-939C04C5AF14}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2068,24 +2240,113 @@
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="115.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
+    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -2185,20 +2446,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.453125" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="115.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" style="4" customWidth="1"/>
+    <col min="3" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -2206,7 +2465,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2215,10 +2474,27 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="7">
+        <v>-27.540875</v>
+      </c>
+      <c r="D2" s="7">
+        <v>152.33902599999999</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2229,10 +2505,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2242,8 +2518,8 @@
     <col min="3" max="3" width="5.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="71.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2252,25 +2528,67 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="7">
+        <v>-27.540875</v>
+      </c>
+      <c r="E2" s="7">
+        <v>152.33902599999999</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="7">
+        <v>-27.540875</v>
+      </c>
+      <c r="E3" s="7">
+        <v>152.33902599999999</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2281,10 +2599,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD1048576"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2293,9 +2611,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2309,7 +2660,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G21" sqref="G21"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2329,44 +2680,108 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E3" s="8"/>
+    </row>
+    <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7">
+        <v>2015</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="5">
+        <v>42145</v>
+      </c>
+      <c r="F2" s="7">
+        <v>150</v>
+      </c>
+      <c r="G2" s="7">
+        <v>50</v>
+      </c>
+      <c r="H2" s="7">
+        <v>250</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
+        <v>2015</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="5">
+        <v>42177</v>
+      </c>
+      <c r="F3" s="7">
+        <v>150</v>
+      </c>
+      <c r="G3" s="7">
+        <v>50</v>
+      </c>
+      <c r="H3" s="7">
+        <v>250</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E4" s="8"/>
@@ -2428,25 +2843,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>